<commit_message>
Revised routing.yml and routing_dev.yml
</commit_message>
<xml_diff>
--- a/skrum_docs/04_SpecificDesign/01_Account_会社新規アカウント作成メール送信画面仕様書_20170712.xlsx
+++ b/skrum_docs/04_SpecificDesign/01_Account_会社新規アカウント作成メール送信画面仕様書_20170712.xlsx
@@ -944,7 +944,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="subsheet!$A$2:$F$5" spid="_x0000_s1033"/>
+                  <a14:cameraTool cellRange="subsheet!$A$2:$F$5" spid="_x0000_s1040"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1384,7 +1384,23 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>新規アカウント作成確認メールを以下のメールアドレスに送信しました。</a:t>
+            <a:t>新規アカウント作成確認メールを以下の</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>E</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>メールアドレスに送信しました。</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800">
             <a:solidFill>
@@ -1400,7 +1416,58 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
+            <a:t>E</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>メールアドレス：</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>sample@gmail.com</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>サブドメイン</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>　：</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>company1</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1414,6 +1481,14 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>E</a:t>
+          </a:r>
+          <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
@@ -1467,7 +1542,23 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>もしメールアドレスを間違えて入力した場合は新規アカウント作成画面に戻り、再度登録を行なってください。</a:t>
+            <a:t>もし</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>E</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>メールアドレスまたは希望サブドメインを間違えて入力した場合は新規アカウント作成画面に戻り、再度登録を行なってください。</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800">
             <a:solidFill>
@@ -1482,15 +1573,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1003300</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>139126</xdr:rowOff>
+      <xdr:colOff>977900</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>189926</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1513,7 +1604,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2794000" y="21005800"/>
+          <a:off x="2768600" y="21818600"/>
           <a:ext cx="1600200" cy="443926"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1526,15 +1617,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1041400</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
+      <xdr:colOff>1003300</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1543,7 +1634,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3302000" y="21031200"/>
+          <a:off x="3263900" y="21844000"/>
           <a:ext cx="660400" cy="381000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">

</xml_diff>